<commit_message>
Edits to our migration data
</commit_message>
<xml_diff>
--- a/Processed Data/refugees_net_by_year_visual.xlsx
+++ b/Processed Data/refugees_net_by_year_visual.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="660" windowWidth="27800" windowHeight="16440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="500" yWindow="620" windowWidth="27800" windowHeight="16440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="refugees_net_by_year_visual.csv" sheetId="1" r:id="rId1"/>
@@ -583,11 +583,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1253326528"/>
-        <c:axId val="-1253312368"/>
+        <c:axId val="-982453456"/>
+        <c:axId val="-982451136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1253326528"/>
+        <c:axId val="-982453456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,7 +630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1253312368"/>
+        <c:crossAx val="-982451136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -638,7 +638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1253312368"/>
+        <c:axId val="-982451136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,6 +658,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -688,7 +689,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1253326528"/>
+        <c:crossAx val="-982453456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8820,11 +8821,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1309118592"/>
-        <c:axId val="-1250369584"/>
+        <c:axId val="-1238212784"/>
+        <c:axId val="-1238198352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1309118592"/>
+        <c:axId val="-1238212784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8867,7 +8868,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1250369584"/>
+        <c:crossAx val="-1238198352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8875,7 +8876,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1250369584"/>
+        <c:axId val="-1238198352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8925,7 +8926,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1309118592"/>
+        <c:crossAx val="-1238212784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>